<commit_message>
take the test accuracy based on the best dev accuracy
</commit_message>
<xml_diff>
--- a/results/time-series-100-99-percent-energy-preserved.xlsx
+++ b/results/time-series-100-99-percent-energy-preserved.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\time-series-machine-leaning\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BDBEF8-4284-4848-A6FC-DA6E0067F2B2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581D7CB8-827A-48CC-883F-AC967F362AB4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="8412" activeTab="3" xr2:uid="{99A84B33-02FC-4241-9637-4ED1B9116C8D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="8412" xr2:uid="{99A84B33-02FC-4241-9637-4ED1B9116C8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="results" sheetId="1" r:id="rId1"/>
-    <sheet name="mnist" sheetId="8" r:id="rId2"/>
-    <sheet name="gpu2" sheetId="6" r:id="rId3"/>
-    <sheet name="100-90" sheetId="7" r:id="rId4"/>
-    <sheet name="p100" sheetId="5" r:id="rId5"/>
-    <sheet name="gpu3" sheetId="2" r:id="rId6"/>
-    <sheet name="50wordsGPU3" sheetId="3" r:id="rId7"/>
+    <sheet name="100-90" sheetId="7" r:id="rId1"/>
+    <sheet name="results" sheetId="1" r:id="rId2"/>
+    <sheet name="mnist" sheetId="8" r:id="rId3"/>
+    <sheet name="gpu2" sheetId="6" r:id="rId4"/>
+    <sheet name="skr-compute1" sheetId="9" r:id="rId5"/>
+    <sheet name="p100" sheetId="5" r:id="rId6"/>
+    <sheet name="gpu3" sheetId="2" r:id="rId7"/>
+    <sheet name="50wordsGPU3" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="344">
   <si>
     <t>Dataset</t>
   </si>
@@ -974,6 +975,102 @@
   </si>
   <si>
     <t>preserve energies: 100</t>
+  </si>
+  <si>
+    <t>ady@skr-compute1:~/code/time-series-ml-experiments/time-series-ml/cnns/nnlib/pytorch_experiments/results$ cat 2018-11-25-00-11-19-843173-ucr</t>
+  </si>
+  <si>
+    <t>preserve energies: 90</t>
+  </si>
+  <si>
+    <t>debug2</t>
+  </si>
+  <si>
+    <t>skr-compute1</t>
+  </si>
+  <si>
+    <t>2018-11-25-00-11-19-843467</t>
+  </si>
+  <si>
+    <t>lr:0.0</t>
+  </si>
+  <si>
+    <t>scheduler_type:SchedulerType.Redu</t>
+  </si>
+  <si>
+    <t>ceLROnPlateau</t>
+  </si>
+  <si>
+    <t>dataset:</t>
+  </si>
+  <si>
+    <t>FT1D</t>
+  </si>
+  <si>
+    <t>visualize:FA</t>
+  </si>
+  <si>
+    <t>LSE</t>
+  </si>
+  <si>
+    <t>parsed_args:Namespace(comp</t>
+  </si>
+  <si>
+    <t>ress_type='STANDARD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dataset='debug2'</t>
+  </si>
+  <si>
+    <t>memory_type='STANDARD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> optimizer_</t>
+  </si>
+  <si>
+    <t>type='ADAM'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> preserve_energies=[90]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> stride_type='ST</t>
+  </si>
+  <si>
+    <t>ANDARD'</t>
+  </si>
+  <si>
+    <t>ady@skr-compute1:~/code/time-series-ml-experiments/time-series-ml/cnns/nnlib/pytorch_experiments/results$ cat 2018-11-25-00-10-59-444233-ucr</t>
+  </si>
+  <si>
+    <t>2018-11-25-00-10-59-444561</t>
+  </si>
+  <si>
+    <t>conv_type:ConvType.</t>
+  </si>
+  <si>
+    <t>visualize:F</t>
+  </si>
+  <si>
+    <t>ALSE</t>
+  </si>
+  <si>
+    <t>parsed_args:Namespace(com</t>
+  </si>
+  <si>
+    <t>press_type='STANDARD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> optimizer</t>
+  </si>
+  <si>
+    <t>_type='ADAM'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> stride_type='</t>
+  </si>
+  <si>
+    <t>STANDARD'</t>
   </si>
 </sst>
 </file>
@@ -1347,6 +1444,668 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175C4BF1-3807-41C7-9FD0-915C0522E87E}">
+  <dimension ref="A1:C87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="29.15625" customWidth="1"/>
+    <col min="2" max="2" width="14.83984375" customWidth="1"/>
+    <col min="3" max="3" width="14.9453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="str">
+        <f>'gpu3'!A6</f>
+        <v>50words</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(results!B3:C3)</f>
+        <v>63.626373626373592</v>
+      </c>
+      <c r="C3">
+        <f>AVERAGE(results!N3:R3)</f>
+        <v>59.780219780219724</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="str">
+        <f>'gpu3'!A12</f>
+        <v>Adiac</v>
+      </c>
+      <c r="B4">
+        <f>AVERAGE(results!B4:C4)</f>
+        <v>80.946291560102253</v>
+      </c>
+      <c r="C4">
+        <f>AVERAGE(results!N4:R4)</f>
+        <v>26.035805626598421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="str">
+        <f>'gpu3'!A18</f>
+        <v>ArrowHead</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(results!B5:C5)</f>
+        <v>83.428571428571402</v>
+      </c>
+      <c r="C5">
+        <f>AVERAGE(results!N5:R5)</f>
+        <v>72.228571428571371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="str">
+        <f>'gpu3'!A24</f>
+        <v>Beef</v>
+      </c>
+      <c r="B6">
+        <f>AVERAGE(results!B6:C6)</f>
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <f>AVERAGE(results!N6:R6)</f>
+        <v>49.333333333333321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="str">
+        <f>'gpu3'!A30</f>
+        <v>BeetleFly</v>
+      </c>
+      <c r="B7">
+        <f>AVERAGE(results!B7:C7)</f>
+        <v>80</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(results!N7:R7)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="str">
+        <f>'gpu3'!A36</f>
+        <v>BirdChicken</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(results!B8:C8)</f>
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(results!N8:R8)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="str">
+        <f>'gpu3'!A45</f>
+        <v>Car</v>
+      </c>
+      <c r="B9">
+        <f>AVERAGE(results!B9:C9)</f>
+        <v>91.6666666666666</v>
+      </c>
+      <c r="C9">
+        <f>AVERAGE(results!N9:R9)</f>
+        <v>60.999999999999979</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="str">
+        <f>'gpu3'!A48</f>
+        <v>CBF</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(results!B10:C10)</f>
+        <v>99.1111111111111</v>
+      </c>
+      <c r="C10">
+        <f>AVERAGE(results!N10:R10)</f>
+        <v>99.466666666666612</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="str">
+        <f>'gpu3'!A57</f>
+        <v>ChlorineConcentration</v>
+      </c>
+      <c r="B11">
+        <f>AVERAGE(results!B11:C11)</f>
+        <v>70.8333333333333</v>
+      </c>
+      <c r="C11">
+        <f>AVERAGE(results!N11:R11)</f>
+        <v>57.546874999999957</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="str">
+        <f>'gpu3'!A60</f>
+        <v>CinC_ECG_torso</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(results!B12:C12)</f>
+        <v>77.246376811594203</v>
+      </c>
+      <c r="C12">
+        <f>'gpu2'!E114</f>
+        <v>54.492753623188399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="str">
+        <f>'gpu3'!A66</f>
+        <v>Coffee</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(results!B13:C13)</f>
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <f>'gpu2'!E115</f>
+        <v>96.428571428571402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14">
+        <f>'gpu3'!E365</f>
+        <v>84</v>
+      </c>
+      <c r="C14">
+        <f>'gpu2'!E116</f>
+        <v>62.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15">
+        <f>'gpu3'!E366</f>
+        <v>77.435897435897402</v>
+      </c>
+      <c r="C15">
+        <f>'gpu2'!E117</f>
+        <v>66.153846153846104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16">
+        <f>'gpu3'!E367</f>
+        <v>77.948717948717899</v>
+      </c>
+      <c r="C16">
+        <f>'gpu2'!E118</f>
+        <v>63.846153846153797</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17">
+        <f>'gpu2'!E119</f>
+        <v>67.179487179487097</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40">
+        <f>'skr-compute1'!E36</f>
+        <v>95.918367346938695</v>
+      </c>
+      <c r="C40">
+        <f>'skr-compute1'!E16</f>
+        <v>94.557823129251702</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41">
+        <f>'skr-compute1'!E37</f>
+        <v>89.066666666666606</v>
+      </c>
+      <c r="C41">
+        <f>'skr-compute1'!E17</f>
+        <v>85.3333333333333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42">
+        <f>'skr-compute1'!E38</f>
+        <v>70.491803278688494</v>
+      </c>
+      <c r="C42">
+        <f>'skr-compute1'!E18</f>
+        <v>75.4098360655737</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43">
+        <f>'skr-compute1'!E39</f>
+        <v>80.821917808219098</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="str">
+        <f>'gpu3'!A81</f>
+        <v>SwedishLeaf</v>
+      </c>
+      <c r="C70">
+        <v>83.68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="str">
+        <f>'gpu3'!A80</f>
+        <v>Symbols</v>
+      </c>
+      <c r="C71">
+        <v>88.040201005025096</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="str">
+        <f>'gpu3'!A79</f>
+        <v>synthetic_control</v>
+      </c>
+      <c r="C72">
+        <v>99.3333333333333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="str">
+        <f>'gpu3'!A78</f>
+        <v>ToeSegmentation1</v>
+      </c>
+      <c r="C73">
+        <v>94.298245614034997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="str">
+        <f>'gpu3'!A77</f>
+        <v>ToeSegmentation2</v>
+      </c>
+      <c r="C74">
+        <v>75.384615384615302</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="str">
+        <f>'gpu3'!A84</f>
+        <v>Wine</v>
+      </c>
+      <c r="B83">
+        <v>66.6666666666666</v>
+      </c>
+      <c r="C83">
+        <v>79.629629629629605</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="str">
+        <f>'gpu3'!A85</f>
+        <v>WordsSynonyms</v>
+      </c>
+      <c r="B84">
+        <v>52.351097178683297</v>
+      </c>
+      <c r="C84">
+        <v>52.5078369905956</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>157</v>
+      </c>
+      <c r="C85">
+        <v>43.093922651933703</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86">
+        <v>74.033149171270694</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>159</v>
+      </c>
+      <c r="C87">
+        <v>76.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88DE2-C050-4555-8254-CCDB84255E3C}">
   <dimension ref="A1:T87"/>
   <sheetViews>
@@ -2912,7 +3671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D571190-9540-45BF-981E-76340F9D56B5}">
   <dimension ref="A1:AN4"/>
   <sheetViews>
@@ -3094,7 +3853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB494C27-D3E5-405E-A38D-EBA7334189A1}">
   <dimension ref="A1:AP137"/>
   <sheetViews>
@@ -4871,633 +5630,750 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175C4BF1-3807-41C7-9FD0-915C0522E87E}">
-  <dimension ref="A1:C87"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB4BAC0-5711-4815-AA2C-74B11E670551}">
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="29.15625" customWidth="1"/>
-    <col min="2" max="2" width="14.83984375" customWidth="1"/>
-    <col min="3" max="3" width="14.9453125" customWidth="1"/>
+    <col min="1" max="1" width="17.9453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="str">
-        <f>'gpu3'!A6</f>
-        <v>50words</v>
-      </c>
-      <c r="B3">
-        <f>AVERAGE(results!B3:C3)</f>
-        <v>63.626373626373592</v>
-      </c>
-      <c r="C3">
-        <f>AVERAGE(results!N3:R3)</f>
-        <v>59.780219780219724</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="str">
-        <f>'gpu3'!A12</f>
-        <v>Adiac</v>
-      </c>
-      <c r="B4">
-        <f>AVERAGE(results!B4:C4)</f>
-        <v>80.946291560102253</v>
-      </c>
-      <c r="C4">
-        <f>AVERAGE(results!N4:R4)</f>
-        <v>26.035805626598421</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="str">
-        <f>'gpu3'!A18</f>
-        <v>ArrowHead</v>
-      </c>
-      <c r="B5">
-        <f>AVERAGE(results!B5:C5)</f>
-        <v>83.428571428571402</v>
-      </c>
-      <c r="C5">
-        <f>AVERAGE(results!N5:R5)</f>
-        <v>72.228571428571371</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="str">
-        <f>'gpu3'!A24</f>
-        <v>Beef</v>
-      </c>
-      <c r="B6">
-        <f>AVERAGE(results!B6:C6)</f>
-        <v>60</v>
-      </c>
-      <c r="C6">
-        <f>AVERAGE(results!N6:R6)</f>
-        <v>49.333333333333321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="str">
-        <f>'gpu3'!A30</f>
-        <v>BeetleFly</v>
-      </c>
-      <c r="B7">
-        <f>AVERAGE(results!B7:C7)</f>
-        <v>80</v>
-      </c>
-      <c r="C7">
-        <f>AVERAGE(results!N7:R7)</f>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="str">
-        <f>'gpu3'!A36</f>
-        <v>BirdChicken</v>
-      </c>
-      <c r="B8">
-        <f>AVERAGE(results!B8:C8)</f>
-        <v>90</v>
-      </c>
-      <c r="C8">
-        <f>AVERAGE(results!N8:R8)</f>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="str">
-        <f>'gpu3'!A45</f>
-        <v>Car</v>
-      </c>
-      <c r="B9">
-        <f>AVERAGE(results!B9:C9)</f>
-        <v>91.6666666666666</v>
-      </c>
-      <c r="C9">
-        <f>AVERAGE(results!N9:R9)</f>
-        <v>60.999999999999979</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="str">
-        <f>'gpu3'!A48</f>
-        <v>CBF</v>
-      </c>
-      <c r="B10">
-        <f>AVERAGE(results!B10:C10)</f>
-        <v>99.1111111111111</v>
-      </c>
-      <c r="C10">
-        <f>AVERAGE(results!N10:R10)</f>
-        <v>99.466666666666612</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="str">
-        <f>'gpu3'!A57</f>
-        <v>ChlorineConcentration</v>
-      </c>
-      <c r="B11">
-        <f>AVERAGE(results!B11:C11)</f>
-        <v>70.8333333333333</v>
-      </c>
-      <c r="C11">
-        <f>AVERAGE(results!N11:R11)</f>
-        <v>57.546874999999957</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="str">
-        <f>'gpu3'!A60</f>
-        <v>CinC_ECG_torso</v>
-      </c>
-      <c r="B12">
-        <f>AVERAGE(results!B12:C12)</f>
-        <v>77.246376811594203</v>
-      </c>
-      <c r="C12">
-        <f>'gpu2'!E114</f>
-        <v>54.492753623188399</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="str">
-        <f>'gpu3'!A66</f>
-        <v>Coffee</v>
-      </c>
-      <c r="B13">
-        <f>AVERAGE(results!B13:C13)</f>
-        <v>100</v>
-      </c>
-      <c r="C13">
-        <f>'gpu2'!E115</f>
-        <v>96.428571428571402</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="e">
+        <f>-fcnn.log</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>321</v>
+      </c>
+      <c r="B7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E7" t="s">
+        <v>270</v>
+      </c>
+      <c r="F7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E8" t="s">
+        <v>274</v>
+      </c>
+      <c r="F8" t="s">
+        <v>275</v>
+      </c>
+      <c r="G8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" t="s">
+        <v>326</v>
+      </c>
+      <c r="D9" t="s">
+        <v>279</v>
+      </c>
+      <c r="E9" t="s">
+        <v>280</v>
+      </c>
+      <c r="F9" t="s">
+        <v>281</v>
+      </c>
+      <c r="G9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" t="s">
+        <v>285</v>
+      </c>
+      <c r="D10" t="s">
+        <v>286</v>
+      </c>
+      <c r="E10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F10" t="s">
+        <v>288</v>
+      </c>
+      <c r="G10" t="s">
+        <v>289</v>
+      </c>
+      <c r="H10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" t="s">
+        <v>293</v>
+      </c>
+      <c r="D11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F11" t="s">
+        <v>296</v>
+      </c>
+      <c r="G11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E12" t="s">
+        <v>301</v>
+      </c>
+      <c r="F12" t="s">
+        <v>302</v>
+      </c>
+      <c r="G12" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13" t="s">
+        <v>304</v>
+      </c>
+      <c r="C13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D13" t="s">
+        <v>306</v>
+      </c>
+      <c r="E13" t="s">
+        <v>307</v>
+      </c>
+      <c r="F13" t="s">
+        <v>308</v>
+      </c>
+      <c r="G13" t="s">
+        <v>309</v>
+      </c>
+      <c r="H13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14">
-        <f>'gpu3'!E365</f>
-        <v>84</v>
-      </c>
-      <c r="C14">
-        <f>'gpu2'!E116</f>
-        <v>62.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15">
-        <f>'gpu3'!E366</f>
-        <v>77.435897435897402</v>
-      </c>
-      <c r="C15">
-        <f>'gpu2'!E117</f>
-        <v>66.153846153846104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="B16">
-        <f>'gpu3'!E367</f>
-        <v>77.948717948717899</v>
+        <v>3.9761442746689003E-2</v>
       </c>
       <c r="C16">
-        <f>'gpu2'!E118</f>
-        <v>63.846153846153797</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>98.507462686567095</v>
+      </c>
+      <c r="D16">
+        <v>0.15565164322060601</v>
+      </c>
+      <c r="E16">
+        <v>94.557823129251702</v>
+      </c>
+      <c r="F16">
+        <v>6116.3665866851798</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>120</v>
+      </c>
+      <c r="B17">
+        <v>0.27755719407399398</v>
       </c>
       <c r="C17">
-        <f>'gpu2'!E119</f>
-        <v>67.179487179487097</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>92.533333333333303</v>
+      </c>
+      <c r="D17">
+        <v>0.42822000885009698</v>
+      </c>
+      <c r="E17">
+        <v>85.3333333333333</v>
+      </c>
+      <c r="F17">
+        <v>35191.678550004901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>121</v>
+      </c>
+      <c r="B18">
+        <v>0.170057128866513</v>
+      </c>
+      <c r="C18">
+        <v>98.3333333333333</v>
+      </c>
+      <c r="D18">
+        <v>0.491844661900254</v>
+      </c>
+      <c r="E18">
+        <v>75.4098360655737</v>
+      </c>
+      <c r="F18">
+        <v>17221.068518877</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="e">
+        <f>-fcnn.log</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>256</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" t="s">
+        <v>257</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>258</v>
+      </c>
+      <c r="H24" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>319</v>
+      </c>
+      <c r="B25" t="s">
+        <v>260</v>
+      </c>
+      <c r="C25" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" t="s">
+        <v>262</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>314</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>264</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>265</v>
+      </c>
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>201</v>
+      </c>
+      <c r="B27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C27" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" t="s">
+        <v>269</v>
+      </c>
+      <c r="E27" t="s">
+        <v>270</v>
+      </c>
+      <c r="F27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>337</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D28" t="s">
+        <v>273</v>
+      </c>
+      <c r="E28" t="s">
+        <v>274</v>
+      </c>
+      <c r="F28" t="s">
+        <v>275</v>
+      </c>
+      <c r="G28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>339</v>
+      </c>
+      <c r="B29" t="s">
+        <v>277</v>
+      </c>
+      <c r="C29" t="s">
+        <v>326</v>
+      </c>
+      <c r="D29" t="s">
+        <v>279</v>
+      </c>
+      <c r="E29" t="s">
+        <v>280</v>
+      </c>
+      <c r="F29" t="s">
+        <v>281</v>
+      </c>
+      <c r="G29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" t="s">
+        <v>284</v>
+      </c>
+      <c r="D30" t="s">
+        <v>285</v>
+      </c>
+      <c r="E30" t="s">
+        <v>286</v>
+      </c>
+      <c r="F30" t="s">
+        <v>287</v>
+      </c>
+      <c r="G30" t="s">
+        <v>288</v>
+      </c>
+      <c r="H30" t="s">
+        <v>289</v>
+      </c>
+      <c r="I30" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>291</v>
+      </c>
+      <c r="B31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C31" t="s">
+        <v>293</v>
+      </c>
+      <c r="D31" t="s">
+        <v>294</v>
+      </c>
+      <c r="E31" t="s">
+        <v>295</v>
+      </c>
+      <c r="F31" t="s">
+        <v>296</v>
+      </c>
+      <c r="G31" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>341</v>
+      </c>
+      <c r="B32" t="s">
+        <v>298</v>
+      </c>
+      <c r="C32" t="s">
+        <v>299</v>
+      </c>
+      <c r="D32" t="s">
+        <v>300</v>
+      </c>
+      <c r="E32" t="s">
+        <v>301</v>
+      </c>
+      <c r="F32" t="s">
+        <v>302</v>
+      </c>
+      <c r="G32" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>343</v>
+      </c>
+      <c r="B33" t="s">
+        <v>304</v>
+      </c>
+      <c r="C33" t="s">
+        <v>305</v>
+      </c>
+      <c r="D33" t="s">
+        <v>306</v>
+      </c>
+      <c r="E33" t="s">
+        <v>307</v>
+      </c>
+      <c r="F33" t="s">
+        <v>308</v>
+      </c>
+      <c r="G33" t="s">
+        <v>309</v>
+      </c>
+      <c r="H33" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>119</v>
+      </c>
+      <c r="B36">
+        <v>4.4163981480384897E-3</v>
+      </c>
+      <c r="C36">
+        <v>100</v>
+      </c>
+      <c r="D36">
+        <v>0.13384296039103</v>
+      </c>
+      <c r="E36">
+        <v>95.918367346938695</v>
+      </c>
+      <c r="F36">
+        <v>4280.9576525688099</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>120</v>
+      </c>
+      <c r="B37">
+        <v>5.4362257798512698E-2</v>
+      </c>
+      <c r="C37">
+        <v>100</v>
+      </c>
+      <c r="D37">
+        <v>0.43035120312372799</v>
+      </c>
+      <c r="E37">
+        <v>89.066666666666606</v>
+      </c>
+      <c r="F37">
+        <v>28117.696531772599</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>121</v>
+      </c>
+      <c r="B38">
+        <v>4.3596070011456801E-2</v>
+      </c>
+      <c r="C38">
+        <v>100</v>
+      </c>
+      <c r="D38">
+        <v>0.68265456840640204</v>
+      </c>
+      <c r="E38">
+        <v>70.491803278688494</v>
+      </c>
+      <c r="F38">
+        <v>4814.0373995304099</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" t="str">
-        <f>'gpu3'!A81</f>
-        <v>SwedishLeaf</v>
-      </c>
-      <c r="C70">
-        <v>83.68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" t="str">
-        <f>'gpu3'!A80</f>
-        <v>Symbols</v>
-      </c>
-      <c r="C71">
-        <v>88.040201005025096</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" t="str">
-        <f>'gpu3'!A79</f>
-        <v>synthetic_control</v>
-      </c>
-      <c r="C72">
-        <v>99.3333333333333</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" t="str">
-        <f>'gpu3'!A78</f>
-        <v>ToeSegmentation1</v>
-      </c>
-      <c r="C73">
-        <v>94.298245614034997</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" t="str">
-        <f>'gpu3'!A77</f>
-        <v>ToeSegmentation2</v>
-      </c>
-      <c r="C74">
-        <v>75.384615384615302</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" t="str">
-        <f>'gpu3'!A84</f>
-        <v>Wine</v>
-      </c>
-      <c r="B83">
-        <v>66.6666666666666</v>
-      </c>
-      <c r="C83">
-        <v>79.629629629629605</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" t="str">
-        <f>'gpu3'!A85</f>
-        <v>WordsSynonyms</v>
-      </c>
-      <c r="B84">
-        <v>52.351097178683297</v>
-      </c>
-      <c r="C84">
-        <v>52.5078369905956</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" t="s">
-        <v>157</v>
-      </c>
-      <c r="C85">
-        <v>43.093922651933703</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" t="s">
-        <v>158</v>
-      </c>
-      <c r="C86">
-        <v>74.033149171270694</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" t="s">
-        <v>159</v>
-      </c>
-      <c r="C87">
-        <v>76.3</v>
+      <c r="B39">
+        <v>7.9881526742662703E-2</v>
+      </c>
+      <c r="C39">
+        <v>100</v>
+      </c>
+      <c r="D39">
+        <v>0.62935330116585497</v>
+      </c>
+      <c r="E39">
+        <v>80.821917808219098</v>
+      </c>
+      <c r="F39">
+        <v>4267.4638450145703</v>
       </c>
     </row>
   </sheetData>
@@ -5505,7 +6381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1274BA09-BD96-435E-A9A6-03CD9E173600}">
   <dimension ref="A1:L72"/>
   <sheetViews>
@@ -6733,7 +7609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC8A15-5897-4C81-BEB9-7876A1902672}">
   <dimension ref="A1:BW367"/>
   <sheetViews>
@@ -13827,7 +14703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEE2090-E0BD-4F84-B877-D58086A9F27D}">
   <dimension ref="A1:AP25"/>
   <sheetViews>

</xml_diff>

<commit_message>
args for conv1d in progress
</commit_message>
<xml_diff>
--- a/results/time-series-100-99-percent-energy-preserved.xlsx
+++ b/results/time-series-100-99-percent-energy-preserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\time-series-machine-leaning\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB318B0E-E94B-4B4C-BC2D-1287756104AF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FE35CB-D5EA-4B72-ACE8-BEAB658147B6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="8412" xr2:uid="{99A84B33-02FC-4241-9637-4ED1B9116C8D}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3996" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="690">
   <si>
     <t>Dataset</t>
   </si>
@@ -2052,6 +2052,66 @@
   </si>
   <si>
     <t>2018-11-24-13-45-08-374716-ucr-fcnn.log                              2018-11-24-13-45-08-375171-dataset-Computers-preserve-energy-90.log</t>
+  </si>
+  <si>
+    <t>2018-11-27-08-44-58-962873</t>
+  </si>
+  <si>
+    <t>epochs:2000</t>
+  </si>
+  <si>
+    <t>learning_rate:0.001</t>
+  </si>
+  <si>
+    <t>weight_decay:0</t>
+  </si>
+  <si>
+    <t>loss_reduction:LossReduction.ELEMENTWISE_MEAN</t>
+  </si>
+  <si>
+    <t>workers:6</t>
+  </si>
+  <si>
+    <t>conv_type:ConvType.STANDARD</t>
+  </si>
+  <si>
+    <t>is_dev_dataset:False</t>
+  </si>
+  <si>
+    <t>dev_percent:100</t>
+  </si>
+  <si>
+    <t>adam_beta1:0.9</t>
+  </si>
+  <si>
+    <t>adam_beta2:0.999</t>
+  </si>
+  <si>
+    <t>parsed_args:Namespace(adam_beta1=0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> adam_beta2=0.999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> compress_type='STANDARD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dev_percent=100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> epochs=2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> learning_rate=0.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> loss_reduction='ELEMENTWISE_MEAN'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> weight_decay=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> workers=6)</t>
   </si>
 </sst>
 </file>
@@ -3980,8 +4040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175C4BF1-3807-41C7-9FD0-915C0522E87E}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8963,10 +9023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC8A15-5897-4C81-BEB9-7876A1902672}">
-  <dimension ref="A1:BW834"/>
+  <dimension ref="A1:CE840"/>
   <sheetViews>
-    <sheetView topLeftCell="A812" workbookViewId="0">
-      <selection activeCell="E823" sqref="E823"/>
+    <sheetView topLeftCell="A824" workbookViewId="0">
+      <selection activeCell="A844" sqref="A844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22578,7 +22638,7 @@
         <v>116085.394322872</v>
       </c>
     </row>
-    <row r="833" spans="1:6">
+    <row r="833" spans="1:83">
       <c r="A833" t="s">
         <v>106</v>
       </c>
@@ -22598,9 +22658,317 @@
         <v>13041.1693787574</v>
       </c>
     </row>
-    <row r="834" spans="1:6">
+    <row r="834" spans="1:83">
       <c r="A834" t="s">
         <v>606</v>
+      </c>
+    </row>
+    <row r="837" spans="1:83">
+      <c r="A837" t="s">
+        <v>17</v>
+      </c>
+      <c r="B837" t="s">
+        <v>18</v>
+      </c>
+      <c r="C837" t="s">
+        <v>19</v>
+      </c>
+      <c r="D837" t="s">
+        <v>20</v>
+      </c>
+      <c r="E837" t="s">
+        <v>21</v>
+      </c>
+      <c r="F837" t="s">
+        <v>670</v>
+      </c>
+      <c r="G837" t="s">
+        <v>23</v>
+      </c>
+      <c r="H837" t="s">
+        <v>24</v>
+      </c>
+      <c r="I837" t="s">
+        <v>671</v>
+      </c>
+      <c r="J837" t="s">
+        <v>672</v>
+      </c>
+      <c r="K837" t="s">
+        <v>673</v>
+      </c>
+      <c r="L837" t="s">
+        <v>81</v>
+      </c>
+      <c r="M837" t="s">
+        <v>257</v>
+      </c>
+      <c r="N837" t="s">
+        <v>29</v>
+      </c>
+      <c r="O837" t="s">
+        <v>30</v>
+      </c>
+      <c r="P837" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q837" t="s">
+        <v>259</v>
+      </c>
+      <c r="R837" t="s">
+        <v>611</v>
+      </c>
+      <c r="S837" t="s">
+        <v>674</v>
+      </c>
+      <c r="T837" t="s">
+        <v>262</v>
+      </c>
+      <c r="U837" t="s">
+        <v>675</v>
+      </c>
+      <c r="V837" t="s">
+        <v>35</v>
+      </c>
+      <c r="W837" t="s">
+        <v>614</v>
+      </c>
+      <c r="X837" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y837" t="s">
+        <v>264</v>
+      </c>
+      <c r="Z837" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA837" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB837" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC837" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD837" t="s">
+        <v>676</v>
+      </c>
+      <c r="AE837" t="s">
+        <v>267</v>
+      </c>
+      <c r="AF837" t="s">
+        <v>268</v>
+      </c>
+      <c r="AG837" t="s">
+        <v>269</v>
+      </c>
+      <c r="AH837" t="s">
+        <v>270</v>
+      </c>
+      <c r="AI837" t="s">
+        <v>271</v>
+      </c>
+      <c r="AJ837" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK837" t="s">
+        <v>272</v>
+      </c>
+      <c r="AL837" t="s">
+        <v>618</v>
+      </c>
+      <c r="AM837" t="s">
+        <v>274</v>
+      </c>
+      <c r="AN837" t="s">
+        <v>275</v>
+      </c>
+      <c r="AO837" t="s">
+        <v>677</v>
+      </c>
+      <c r="AP837" t="s">
+        <v>678</v>
+      </c>
+      <c r="AQ837" t="s">
+        <v>679</v>
+      </c>
+      <c r="AR837" t="s">
+        <v>680</v>
+      </c>
+      <c r="AS837" t="s">
+        <v>681</v>
+      </c>
+      <c r="AT837" t="s">
+        <v>682</v>
+      </c>
+      <c r="AU837" t="s">
+        <v>683</v>
+      </c>
+      <c r="AV837" t="s">
+        <v>622</v>
+      </c>
+      <c r="AW837" t="s">
+        <v>623</v>
+      </c>
+      <c r="AX837" t="s">
+        <v>684</v>
+      </c>
+      <c r="AY837" t="s">
+        <v>279</v>
+      </c>
+      <c r="AZ837" t="s">
+        <v>685</v>
+      </c>
+      <c r="BA837" t="s">
+        <v>281</v>
+      </c>
+      <c r="BB837" t="s">
+        <v>282</v>
+      </c>
+      <c r="BC837" t="s">
+        <v>283</v>
+      </c>
+      <c r="BD837" t="s">
+        <v>627</v>
+      </c>
+      <c r="BE837" t="s">
+        <v>284</v>
+      </c>
+      <c r="BF837" t="s">
+        <v>686</v>
+      </c>
+      <c r="BG837" t="s">
+        <v>285</v>
+      </c>
+      <c r="BH837" t="s">
+        <v>687</v>
+      </c>
+      <c r="BI837" t="s">
+        <v>630</v>
+      </c>
+      <c r="BJ837" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK837" t="s">
+        <v>631</v>
+      </c>
+      <c r="BL837" t="s">
+        <v>291</v>
+      </c>
+      <c r="BM837" t="s">
+        <v>292</v>
+      </c>
+      <c r="BN837" t="s">
+        <v>293</v>
+      </c>
+      <c r="BO837" t="s">
+        <v>294</v>
+      </c>
+      <c r="BP837" t="s">
+        <v>295</v>
+      </c>
+      <c r="BQ837" t="s">
+        <v>296</v>
+      </c>
+      <c r="BR837" t="s">
+        <v>297</v>
+      </c>
+      <c r="BS837" t="s">
+        <v>298</v>
+      </c>
+      <c r="BT837" t="s">
+        <v>299</v>
+      </c>
+      <c r="BU837" t="s">
+        <v>300</v>
+      </c>
+      <c r="BV837" t="s">
+        <v>301</v>
+      </c>
+      <c r="BW837" t="s">
+        <v>302</v>
+      </c>
+      <c r="BX837" t="s">
+        <v>303</v>
+      </c>
+      <c r="BY837" t="s">
+        <v>304</v>
+      </c>
+      <c r="BZ837" t="s">
+        <v>305</v>
+      </c>
+      <c r="CA837" t="s">
+        <v>306</v>
+      </c>
+      <c r="CB837" t="s">
+        <v>307</v>
+      </c>
+      <c r="CC837" t="s">
+        <v>688</v>
+      </c>
+      <c r="CD837" t="s">
+        <v>689</v>
+      </c>
+      <c r="CE837" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="838" spans="1:83">
+      <c r="A838" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="839" spans="1:83">
+      <c r="A839" t="s">
+        <v>73</v>
+      </c>
+      <c r="B839" t="s">
+        <v>52</v>
+      </c>
+      <c r="C839" t="s">
+        <v>53</v>
+      </c>
+      <c r="D839" t="s">
+        <v>636</v>
+      </c>
+      <c r="E839" t="s">
+        <v>637</v>
+      </c>
+      <c r="F839" t="s">
+        <v>54</v>
+      </c>
+      <c r="G839" t="s">
+        <v>55</v>
+      </c>
+      <c r="H839" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="840" spans="1:83">
+      <c r="A840" t="s">
+        <v>57</v>
+      </c>
+      <c r="B840">
+        <v>2.0883617591526699E-2</v>
+      </c>
+      <c r="C840">
+        <v>94.4444444444444</v>
+      </c>
+      <c r="D840" t="s">
+        <v>638</v>
+      </c>
+      <c r="E840" t="s">
+        <v>638</v>
+      </c>
+      <c r="F840">
+        <v>8.3984635033450203E-2</v>
+      </c>
+      <c r="G840">
+        <v>63.736263736263702</v>
+      </c>
+      <c r="H840">
+        <v>2437.5520927906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
step size = batch size for conv1
</commit_message>
<xml_diff>
--- a/results/time-series-100-99-percent-energy-preserved.xlsx
+++ b/results/time-series-100-99-percent-energy-preserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\time-series-machine-leaning\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3AA84D-14D4-468B-A9DD-30905447CAD4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C55BC5-D2B8-4D0D-817C-94031143DED6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="8412" activeTab="1" xr2:uid="{99A84B33-02FC-4241-9637-4ED1B9116C8D}"/>
   </bookViews>
@@ -3271,7 +3271,6 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
@@ -4549,7 +4548,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>graph!$C$1:$C$47</c15:sqref>
@@ -4704,7 +4703,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>graph!$G$1:$G$47</c15:sqref>
@@ -4856,7 +4855,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-D313-4F00-92F8-3B836D7DF97A}"/>
                   </c:ext>
@@ -8438,15 +8437,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>36194</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12379,7 +12378,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="M62" sqref="M62"/>
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12466,15 +12465,15 @@
         <v>3.1090373280943058</v>
       </c>
       <c r="F4">
-        <f>$A4/$G$1*100</f>
+        <f t="shared" ref="F4:G23" si="1">$A4/$G$1*100</f>
         <v>4.4444444444444446</v>
       </c>
       <c r="G4">
-        <f>$A4/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>4.4444444444444446</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H47" si="1">$C4</f>
+        <f t="shared" ref="H4:H47" si="2">$C4</f>
         <v>80.946291560102253</v>
       </c>
     </row>
@@ -12499,15 +12498,15 @@
         <v>1.1550632911392411</v>
       </c>
       <c r="F5">
-        <f>$A5/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>6.666666666666667</v>
       </c>
       <c r="G5">
-        <f>$A5/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>6.666666666666667</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.428571428571402</v>
       </c>
     </row>
@@ -12532,15 +12531,15 @@
         <v>1.2162162162162165</v>
       </c>
       <c r="F6">
-        <f>$A6/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>8.8888888888888893</v>
       </c>
       <c r="G6">
-        <f>$A6/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>8.8888888888888893</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
@@ -12565,15 +12564,15 @@
         <v>0.85106382978723405</v>
       </c>
       <c r="F7">
-        <f>$A7/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
       <c r="G7">
-        <f>$A7/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
     </row>
@@ -12598,15 +12597,15 @@
         <v>1.139240506329114</v>
       </c>
       <c r="F8">
-        <f>$A8/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>13.333333333333334</v>
       </c>
       <c r="G8">
-        <f>$A8/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>13.333333333333334</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
@@ -12631,15 +12630,15 @@
         <v>1.5027322404371579</v>
       </c>
       <c r="F9">
-        <f>$A9/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>15.555555555555555</v>
       </c>
       <c r="G9">
-        <f>$A9/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>15.555555555555555</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91.6666666666666</v>
       </c>
     </row>
@@ -12664,15 +12663,15 @@
         <v>0.99642537980339629</v>
       </c>
       <c r="F10">
-        <f>$A10/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>17.777777777777779</v>
       </c>
       <c r="G10">
-        <f>$A10/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>17.777777777777779</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99.1111111111111</v>
       </c>
     </row>
@@ -12697,15 +12696,15 @@
         <v>1.230880622680786</v>
       </c>
       <c r="F11">
-        <f>$A11/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="G11">
-        <f>$A11/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70.8333333333333</v>
       </c>
     </row>
@@ -12730,15 +12729,15 @@
         <v>1.417553191489362</v>
       </c>
       <c r="F12">
-        <f>$A12/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>22.222222222222221</v>
       </c>
       <c r="G12">
-        <f>$A12/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>22.222222222222221</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77.246376811594203</v>
       </c>
     </row>
@@ -12763,15 +12762,15 @@
         <v>1.0370370370370374</v>
       </c>
       <c r="F13">
-        <f>$A13/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>24.444444444444443</v>
       </c>
       <c r="G13">
-        <f>$A13/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>24.444444444444443</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -12795,15 +12794,15 @@
         <v>1.2688821752265864</v>
       </c>
       <c r="F14">
-        <f>$A14/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>26.666666666666668</v>
       </c>
       <c r="G14">
-        <f>$A14/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>26.666666666666668</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
     </row>
@@ -12827,15 +12826,15 @@
         <v>1.1660231660231666</v>
       </c>
       <c r="F15">
-        <f>$A15/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>28.888888888888886</v>
       </c>
       <c r="G15">
-        <f>$A15/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>28.888888888888886</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77.435897435897402</v>
       </c>
     </row>
@@ -12859,15 +12858,15 @@
         <v>1.2587991718426499</v>
       </c>
       <c r="F16">
-        <f>$A16/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>31.111111111111111</v>
       </c>
       <c r="G16">
-        <f>$A16/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>31.111111111111111</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77.948717948717899</v>
       </c>
     </row>
@@ -12891,15 +12890,15 @@
         <v>1.1590909090909087</v>
       </c>
       <c r="F17">
-        <f>$A17/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>33.333333333333329</v>
       </c>
       <c r="G17">
-        <f>$A17/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>33.333333333333329</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78.461538461538396</v>
       </c>
     </row>
@@ -12923,15 +12922,15 @@
         <v>1.3676470588235294</v>
       </c>
       <c r="F18">
-        <f>$A18/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>35.555555555555557</v>
       </c>
       <c r="G18">
-        <f>$A18/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>35.555555555555557</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91.176470588235205</v>
       </c>
     </row>
@@ -12955,15 +12954,15 @@
         <v>1.0626959247648904</v>
       </c>
       <c r="F19">
-        <f>$A19/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>37.777777777777779</v>
       </c>
       <c r="G19">
-        <f>$A19/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>37.777777777777779</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84.75</v>
       </c>
     </row>
@@ -12987,15 +12986,15 @@
         <v>1.0774336283185837</v>
       </c>
       <c r="F20">
-        <f>$A20/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="G20">
-        <f>$A20/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81.1666666666666</v>
       </c>
     </row>
@@ -13019,15 +13018,15 @@
         <v>1.0707070707070707</v>
       </c>
       <c r="F21">
-        <f>$A21/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>42.222222222222221</v>
       </c>
       <c r="G21">
-        <f>$A21/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>42.222222222222221</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79.5</v>
       </c>
     </row>
@@ -13051,15 +13050,15 @@
         <v>1.0286885245901645</v>
       </c>
       <c r="F22">
-        <f>$A22/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>44.444444444444443</v>
       </c>
       <c r="G22">
-        <f>$A22/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>44.444444444444443</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77.950310559006198</v>
       </c>
     </row>
@@ -13083,15 +13082,15 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <f>$A23/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>46.666666666666664</v>
       </c>
       <c r="G23">
-        <f>$A23/$G$1*100</f>
+        <f t="shared" si="1"/>
         <v>46.666666666666664</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
     </row>
@@ -13115,15 +13114,15 @@
         <v>0.99599340089559352</v>
       </c>
       <c r="F24">
-        <f>$A24/$G$1*100</f>
+        <f t="shared" ref="F24:G47" si="3">$A24/$G$1*100</f>
         <v>48.888888888888886</v>
       </c>
       <c r="G24">
-        <f>$A24/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>48.888888888888886</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>93.911111111111097</v>
       </c>
     </row>
@@ -13147,15 +13146,15 @@
         <v>0.98941176470588221</v>
       </c>
       <c r="F25">
-        <f>$A25/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>51.111111111111107</v>
       </c>
       <c r="G25">
-        <f>$A25/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>51.111111111111107</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97.677119628339099</v>
       </c>
     </row>
@@ -13179,15 +13178,15 @@
         <v>1.1561004784688989</v>
       </c>
       <c r="F26">
-        <f>$A26/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>53.333333333333336</v>
       </c>
       <c r="G26">
-        <f>$A26/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>53.333333333333336</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75.204253663597399</v>
       </c>
     </row>
@@ -13211,15 +13210,15 @@
         <v>1.1930091185410325</v>
       </c>
       <c r="F27">
-        <f>$A27/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>55.555555555555557</v>
       </c>
       <c r="G27">
-        <f>$A27/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>55.555555555555557</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.899408284023593</v>
       </c>
     </row>
@@ -13243,15 +13242,15 @@
         <v>1.0124999999999995</v>
       </c>
       <c r="F28">
-        <f>$A28/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>57.777777777777771</v>
       </c>
       <c r="G28">
-        <f>$A28/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>57.777777777777771</v>
       </c>
       <c r="H28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.045454545454504</v>
       </c>
     </row>
@@ -13275,15 +13274,15 @@
         <v>0.99370409233997936</v>
       </c>
       <c r="F29">
-        <f>$A29/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="G29">
-        <f>$A29/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="H29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.390243902438996</v>
       </c>
     </row>
@@ -13307,15 +13306,15 @@
         <v>1.6249999999999996</v>
       </c>
       <c r="F30">
-        <f>$A30/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>62.222222222222221</v>
       </c>
       <c r="G30">
-        <f>$A30/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>62.222222222222221</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96.571428571428498</v>
       </c>
     </row>
@@ -13339,15 +13338,15 @@
         <v>1.0771503611293509</v>
       </c>
       <c r="F31">
-        <f>$A31/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>64.444444444444443</v>
       </c>
       <c r="G31">
-        <f>$A31/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>64.444444444444443</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91.113579561232996</v>
       </c>
     </row>
@@ -13371,15 +13370,15 @@
         <v>1.0143884892086321</v>
       </c>
       <c r="F32">
-        <f>$A32/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>66.666666666666657</v>
       </c>
       <c r="G32">
-        <f>$A32/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>66.666666666666657</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>95.918367346938695</v>
       </c>
     </row>
@@ -13403,15 +13402,15 @@
         <v>1.0437499999999997</v>
       </c>
       <c r="F33">
-        <f>$A33/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>68.888888888888886</v>
       </c>
       <c r="G33">
-        <f>$A33/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>68.888888888888886</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89.066666666666606</v>
       </c>
     </row>
@@ -13435,15 +13434,15 @@
         <v>0.93478260869565266</v>
       </c>
       <c r="F34">
-        <f>$A34/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>71.111111111111114</v>
       </c>
       <c r="G34">
-        <f>$A34/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>71.111111111111114</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70.491803278688494</v>
       </c>
     </row>
@@ -13467,15 +13466,15 @@
         <v>1.0172413793103443</v>
       </c>
       <c r="F35">
-        <f>$A35/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>73.333333333333329</v>
       </c>
       <c r="G35">
-        <f>$A35/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>73.333333333333329</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80.821917808219098</v>
       </c>
     </row>
@@ -13499,15 +13498,15 @@
         <v>0.97419354838709604</v>
       </c>
       <c r="F36">
-        <f>$A36/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>75.555555555555557</v>
       </c>
       <c r="G36">
-        <f>$A36/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>75.555555555555557</v>
       </c>
       <c r="H36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90.149253731343194</v>
       </c>
     </row>
@@ -13531,15 +13530,15 @@
         <v>1.0833333333333333</v>
       </c>
       <c r="F37">
-        <f>$A37/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>77.777777777777786</v>
       </c>
       <c r="G37">
-        <f>$A37/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>77.777777777777786</v>
       </c>
       <c r="H37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
     </row>
@@ -13563,15 +13562,15 @@
         <v>1.0626118067978543</v>
       </c>
       <c r="F38">
-        <f>$A38/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="G38">
-        <f>$A38/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="H38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78.157894736842096</v>
       </c>
     </row>
@@ -13595,15 +13594,15 @@
         <v>1.0724137931034483</v>
       </c>
       <c r="F39">
-        <f>$A39/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>82.222222222222214</v>
       </c>
       <c r="G39">
-        <f>$A39/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>82.222222222222214</v>
       </c>
       <c r="H39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77.75</v>
       </c>
     </row>
@@ -13627,15 +13626,15 @@
         <v>1.1503267973856197</v>
       </c>
       <c r="F40">
-        <f>$A40/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>84.444444444444443</v>
       </c>
       <c r="G40">
-        <f>$A40/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>84.444444444444443</v>
       </c>
       <c r="H40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58.6666666666666</v>
       </c>
     </row>
@@ -13659,15 +13658,15 @@
         <v>0.9728682170542633</v>
       </c>
       <c r="F41">
-        <f>$A41/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>86.666666666666671</v>
       </c>
       <c r="G41">
-        <f>$A41/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>86.666666666666671</v>
       </c>
       <c r="H41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62.907268170426001</v>
       </c>
     </row>
@@ -13691,15 +13690,15 @@
         <v>1.0355871886120993</v>
       </c>
       <c r="F42">
-        <f>$A42/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>88.888888888888886</v>
       </c>
       <c r="G42">
-        <f>$A42/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>88.888888888888886</v>
       </c>
       <c r="H42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.971246006389705</v>
       </c>
     </row>
@@ -13723,15 +13722,15 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <f>$A43/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>91.111111111111114</v>
       </c>
       <c r="G43">
-        <f>$A43/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>91.111111111111114</v>
       </c>
       <c r="H43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
@@ -13753,15 +13752,15 @@
         <v>0.99534883720930312</v>
       </c>
       <c r="F44">
-        <f>$A44/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>93.333333333333329</v>
       </c>
       <c r="G44">
-        <f>$A44/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>93.333333333333329</v>
       </c>
       <c r="H44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>93.859649122806999</v>
       </c>
     </row>
@@ -13783,15 +13782,15 @@
         <v>1.2142857142857151</v>
       </c>
       <c r="F45">
-        <f>$A45/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>95.555555555555557</v>
       </c>
       <c r="G45">
-        <f>$A45/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>95.555555555555557</v>
       </c>
       <c r="H45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91.538461538461505</v>
       </c>
     </row>
@@ -13814,15 +13813,15 @@
         <v>0.83720930232558077</v>
       </c>
       <c r="F46">
-        <f>$A46/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>97.777777777777771</v>
       </c>
       <c r="G46">
-        <f>$A46/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>97.777777777777771</v>
       </c>
       <c r="H46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66.6666666666666</v>
       </c>
     </row>
@@ -13845,15 +13844,15 @@
         <v>0.99701492537313285</v>
       </c>
       <c r="F47">
-        <f>$A47/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="G47">
-        <f>$A47/$G$1*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="H47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52.351097178683297</v>
       </c>
     </row>

</xml_diff>